<commit_message>
update content list and word list
</commit_message>
<xml_diff>
--- a/assets/xlsx/00_content_list.xlsx
+++ b/assets/xlsx/00_content_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\github_personal\whdrns2013.github.io\assets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B347A29-A7D6-4F23-91F2-349C152C030A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBB602D-F8C3-401E-9471-398ACFD3AFEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="84">
   <si>
     <t>post code</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -194,6 +194,186 @@
   </si>
   <si>
     <t>방송통신대 2024-02 머신러닝 시스템 4강</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                   </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>셸의 개념과 기본적인 사용법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>셸 명령어의 종류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>셸 명령 히스토리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>셸 명령에서의 특수문자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>셸 변수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방송통신대 2024-02 UNIX 시스템 3강</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리눅스 파일 시스템</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리눅스 파일 및 디렉터리 관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리눅스 파일 및 디렉터리 접근권한 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리눅스 파일 내용 확인과 출력하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방송통신대 2024-02 UNIX 시스템 4강</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리눅스의 부팅 과정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리눅스 초기화 데몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>systemd, 유닛, 시스템 서비스의 관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리눅스 시스템의 종료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방송통신대 2024-02 UNIX 시스템 5강</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리눅스 사용자 계정과 파일의 접근 권한 (앞쪽 뒤쪽 혼합)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리눅스 su, sudo 명령</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리눅스 사용자 및 그룹 계정 관리 파일 (중간중간)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리눅스 그룹 계정의 관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리눅스 사용자 계정 생성과 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방송통신대 2024-02 UNIX 시스템 6강</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리눅스 텍스트 편집기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리눅스에서 텍스트 파일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vi 편집기 사용법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리눅스 파일 찾기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리눅스 문자열 검색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방송통신대 2024-02 UNIX 시스템 7강</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방송통신대 2024-02 머신러닝 시스템 1강</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>머신러닝의 개념 (5-13)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>머신러닝 시스템 개발 과정 (14-16)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>머신러닝의 종류와 대상 주제 (27-41, 대략적으로만 설명하면 됨. 이전 내용은 패스해도 됨)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>머신러닝의 유형 (44, 지도, 비지도…)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분류 모델 - 개념</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분류 모델 - 베이즈 분류기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분류 모델 - K-최근접이웃 분류기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분류 모델 - 분류 모델의 종류 (35p)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방송통신대 2024-02 머신러닝 시스템 2강</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회귀 모델 - 개념</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회귀 모델 - 회귀 모델의 종류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회귀 모델 - 선형 회귀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회귀 모델 - 선형 회귀의 확정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회귀 모델 - 로지스틱 회귀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방송통신대 2024-02 머신러닝 시스템 3강</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -581,11 +761,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -638,280 +818,786 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="F23" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F9" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F6" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>